<commit_message>
end of week update for sprint and product backlogs
</commit_message>
<xml_diff>
--- a/Sprint 1 Documentation/ProductBacklog.xlsx
+++ b/Sprint 1 Documentation/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_151a\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1283\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC5F5CD-5E21-4007-ADD6-BEC21A1F76D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2A953D5-581D-4208-8260-99C0E2A692A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>User Story ID</t>
   </si>
@@ -75,12 +75,15 @@
     <t>28/1/2020</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>As a customer, I can search based on code</t>
+  </si>
+  <si>
     <t>In-progress</t>
   </si>
   <si>
-    <t>As a customer, I can search based on code</t>
-  </si>
-  <si>
     <t>As a customer, I can search based on procedure</t>
   </si>
   <si>
@@ -96,40 +99,46 @@
     <t>As a customer, I can view details of a search result in the list</t>
   </si>
   <si>
+    <t>PUSHED TO SPRINT 2</t>
+  </si>
+  <si>
+    <t>As a customer, I can sort search results based on price</t>
+  </si>
+  <si>
+    <t>As a customer, I can sort search results based on location</t>
+  </si>
+  <si>
+    <t>As a customer, I can view details of a search result on a map</t>
+  </si>
+  <si>
+    <t>As a customer, I can set a price range for my search</t>
+  </si>
+  <si>
+    <t>As a customer, I can set a distance range for my search</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>As a customer, I can view service provider information page</t>
+  </si>
+  <si>
+    <t>As a customer, I can sort search results based on "best match"</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>As an admin, I can login to an admin account</t>
+  </si>
+  <si>
     <t>Not Started</t>
   </si>
   <si>
-    <t>As a customer, I can sort search results based on price</t>
-  </si>
-  <si>
-    <t>As a customer, I can sort search results based on location</t>
-  </si>
-  <si>
-    <t>As a customer, I can view details of a search result on a map</t>
-  </si>
-  <si>
-    <t>As a customer, I can set a price range for my search</t>
-  </si>
-  <si>
-    <t>As a customer, I can set a distance range for my search</t>
-  </si>
-  <si>
-    <t>As a customer, I can view service provider information page</t>
-  </si>
-  <si>
-    <t>As a customer, I can sort search results based on "best match"</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>As an admin, I can login to an admin account</t>
-  </si>
-  <si>
     <t>As an admin, I can add a new medical centre</t>
   </si>
   <si>
-    <t>As an admin, I can add a medical centre</t>
+    <t>As an admin, I can remove a medical centre</t>
   </si>
   <si>
     <t>As an admin, I can edit details of a medical centre</t>
@@ -139,9 +148,6 @@
   </si>
   <si>
     <t>As a customer, I can rate a medical centre</t>
-  </si>
-  <si>
-    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -559,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ25"/>
+  <dimension ref="A1:BJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E13" sqref="E13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,14 +576,15 @@
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="55.140625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -606,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1">
+    <row r="2" spans="1:11" s="8" customFormat="1">
       <c r="A2" s="7"/>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -618,7 +625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>14</v>
       </c>
@@ -638,14 +645,14 @@
         <v>3</v>
       </c>
       <c r="H3" s="3">
-        <f>(F3/G3)</f>
+        <f t="shared" ref="H3:H16" si="0">(F3/G3)</f>
         <v>3.3333333333333335</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -655,6 +662,9 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
       <c r="F4">
         <v>10</v>
       </c>
@@ -662,22 +672,25 @@
         <v>4</v>
       </c>
       <c r="H4" s="1">
-        <f>(F4/G4)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -686,22 +699,25 @@
         <v>4</v>
       </c>
       <c r="H5" s="1">
-        <f>(F5/G5)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
       </c>
       <c r="F6">
         <v>9</v>
@@ -710,22 +726,25 @@
         <v>9</v>
       </c>
       <c r="H6" s="1">
-        <f>(F6/G6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -734,22 +753,25 @@
         <v>1</v>
       </c>
       <c r="H7" s="1">
-        <f>(F7/G7)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
       </c>
       <c r="F8">
         <v>8</v>
@@ -758,22 +780,25 @@
         <v>7</v>
       </c>
       <c r="H8" s="1">
-        <f>(F8/G8)</f>
+        <f t="shared" si="0"/>
         <v>1.1428571428571428</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -782,23 +807,26 @@
         <v>2</v>
       </c>
       <c r="H9" s="1">
-        <f>(F9/G9)</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
       <c r="F10">
         <v>6</v>
       </c>
@@ -806,23 +834,26 @@
         <v>2</v>
       </c>
       <c r="H10" s="1">
-        <f>(F10/G10)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
       <c r="F11">
         <v>6</v>
       </c>
@@ -830,23 +861,26 @@
         <v>2</v>
       </c>
       <c r="H11" s="1">
-        <f>(F11/G11)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
       <c r="F12">
         <v>5</v>
       </c>
@@ -854,22 +888,25 @@
         <v>7</v>
       </c>
       <c r="H12" s="1">
-        <f>(F12/G12)</f>
+        <f t="shared" si="0"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -878,23 +915,26 @@
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <f>(F13/G13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
       <c r="F14">
         <v>4</v>
       </c>
@@ -902,22 +942,28 @@
         <v>1</v>
       </c>
       <c r="H14" s="1">
-        <f>(F14/G14)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
       </c>
       <c r="F15" s="5">
         <v>4</v>
@@ -926,23 +972,26 @@
         <v>3</v>
       </c>
       <c r="H15" s="1">
-        <f>(F15/G15)</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
       <c r="F16">
         <v>2</v>
       </c>
@@ -950,11 +999,11 @@
         <v>4</v>
       </c>
       <c r="H16" s="1">
-        <f>(F16/G16)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:62" s="6" customFormat="1">
@@ -990,7 +1039,7 @@
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D19" s="11">
         <v>43892</v>
@@ -1057,50 +1106,56 @@
       <c r="BJ19" s="10"/>
     </row>
     <row r="20" spans="1:62">
-      <c r="A20" s="2">
-        <v>17</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="2">
-        <v>3</v>
-      </c>
-      <c r="G20" s="2">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:H21" si="1">(F20/G20)</f>
+        <v>3.5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21">
         <v>5</v>
       </c>
-      <c r="H20" s="3">
-        <f>(F20/G20)</f>
-        <v>0.6</v>
-      </c>
-      <c r="I20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:62">
-      <c r="A21" s="2">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="2">
-        <v>3</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>7</v>
       </c>
-      <c r="H21" s="3">
-        <f>(F21/G21)</f>
-        <v>0.42857142857142855</v>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:62">
       <c r="A22" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>32</v>
@@ -1109,86 +1164,162 @@
         <v>3</v>
       </c>
       <c r="G22" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H22" s="3">
-        <f>(F22/G22)</f>
-        <v>0.42857142857142855</v>
+        <f t="shared" ref="H22:H31" si="2">(F22/G22)</f>
+        <v>0.6</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:62">
       <c r="A23" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F23" s="2">
         <v>3</v>
       </c>
       <c r="G23" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" s="3">
-        <f>(F23/G23)</f>
-        <v>0.375</v>
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:62">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>8</v>
-      </c>
-      <c r="H24" s="1">
-        <f>(F24/G24)</f>
-        <v>0.125</v>
+      <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2">
+        <v>7</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I24" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:62">
       <c r="A25" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F25" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G25" s="2">
         <v>8</v>
       </c>
       <c r="H25" s="3">
-        <f>(F25/G25)</f>
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="I25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:62">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" ref="H26" si="3">(F26/G26)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:62">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
-      <c r="I25" t="s">
-        <v>21</v>
-      </c>
+      <c r="I27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:62">
+      <c r="A28" s="2">
+        <v>15</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>8</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="I28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:62">
+      <c r="D29" s="4"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:62">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:62">
+      <c r="H31" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:I25">
-    <sortCondition descending="1" ref="F20:F25"/>
-    <sortCondition ref="G20:G25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:I28">
+    <sortCondition descending="1" ref="F22:F28"/>
+    <sortCondition ref="G22:G28"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2 I18:I19 I26:I1048576" xr:uid="{1E6226B8-A8D1-4D7A-9B0F-FAA90AAF118D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2 I32:I1048576 I18:I19" xr:uid="{1E6226B8-A8D1-4D7A-9B0F-FAA90AAF118D}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1200,7 +1331,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I16 I20:I25</xm:sqref>
+          <xm:sqref>I3:I16 I20:I31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1221,17 +1352,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final reconfiguration of documentation for sprint 1 for final review
</commit_message>
<xml_diff>
--- a/Sprint 1 Documentation/ProductBacklog.xlsx
+++ b/Sprint 1 Documentation/ProductBacklog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1283\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni - gitfolder\Agile-Software-Development\Sprint 1 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2A953D5-581D-4208-8260-99C0E2A692A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8124FB-4A06-41BB-BFAF-7DD6E367DC5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,23 +568,23 @@
   <dimension ref="A1:BJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E15"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -613,7 +613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1">
+    <row r="2" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -625,7 +625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>14</v>
       </c>
@@ -652,7 +652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -676,10 +676,10 @@
         <v>2.5</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -703,10 +703,10 @@
         <v>2.5</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -730,10 +730,10 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
@@ -757,10 +757,10 @@
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9</v>
       </c>
@@ -784,10 +784,10 @@
         <v>1.1428571428571428</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -814,7 +814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -838,10 +838,10 @@
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -865,10 +865,10 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>13</v>
       </c>
@@ -895,7 +895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -919,10 +919,10 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -946,13 +946,13 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>16</v>
       </c>
@@ -976,10 +976,10 @@
         <v>1.3333333333333333</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1003,10 +1003,10 @@
         <v>0.5</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:62" s="6" customFormat="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:62" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:62" s="12" customFormat="1">
+    <row r="19" spans="1:62" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="9" t="s">
@@ -1105,7 +1105,7 @@
       <c r="BI19" s="10"/>
       <c r="BJ19" s="10"/>
     </row>
-    <row r="20" spans="1:62">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:62">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>13</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:62">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>17</v>
       </c>
@@ -1167,14 +1167,14 @@
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" ref="H22:H31" si="2">(F22/G22)</f>
+        <f t="shared" ref="H22:H28" si="2">(F22/G22)</f>
         <v>0.6</v>
       </c>
       <c r="I22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:62">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:62">
+    <row r="24" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:62">
+    <row r="25" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>18</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:62">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:62">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:62">
+    <row r="28" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>15</v>
       </c>
@@ -1303,14 +1303,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:62">
+    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
       <c r="D29" s="4"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:62">
+    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:62">
+    <row r="31" spans="1:62" x14ac:dyDescent="0.3">
       <c r="H31" s="1"/>
     </row>
   </sheetData>
@@ -1331,7 +1331,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I16 I20:I31</xm:sqref>
+          <xm:sqref>I20:I31 I3:I16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1345,22 +1345,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
sprint backlog updated for day 2
</commit_message>
<xml_diff>
--- a/Sprint 1 Documentation/ProductBacklog.xlsx
+++ b/Sprint 1 Documentation/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni - gitfolder\Agile-Software-Development\Sprint 1 Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni - gitfolder\Agile-Software-Development\Sprint 2 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8124FB-4A06-41BB-BFAF-7DD6E367DC5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAA1562-473F-473D-90EE-2E17E9EF21F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
   <si>
     <t>User Story ID</t>
   </si>
@@ -148,13 +146,28 @@
   </si>
   <si>
     <t>As a customer, I can rate a medical centre</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>code - the medical code for the required procedure</t>
+  </si>
+  <si>
+    <t>procedure - search using key words to find the procedure required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rating - a customer left review/rating </t>
+  </si>
+  <si>
+    <t>best match - a self made formula comparing price to distance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +185,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -251,6 +273,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ31"/>
+  <dimension ref="A1:BJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,7 +930,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -919,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -933,7 +957,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -946,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
@@ -1003,7 +1027,7 @@
         <v>0.5</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:62" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1122,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" ref="H20:H21" si="1">(F20/G20)</f>
+        <f t="shared" ref="H20:H30" si="1">(F20/G20)</f>
         <v>3.5</v>
       </c>
       <c r="I20" t="s">
@@ -1154,63 +1178,71 @@
       </c>
     </row>
     <row r="22" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="2">
-        <v>3</v>
-      </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
-      <c r="H22" s="3">
-        <f t="shared" ref="H22:H28" si="2">(F22/G22)</f>
-        <v>0.6</v>
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>19</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="2">
-        <v>3</v>
-      </c>
-      <c r="G23" s="2">
-        <v>7</v>
-      </c>
-      <c r="H23" s="3">
-        <f t="shared" si="2"/>
-        <v>0.42857142857142855</v>
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F24" s="2">
         <v>3</v>
       </c>
       <c r="G24" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="2"/>
-        <v>0.42857142857142855</v>
+        <f t="shared" si="1"/>
+        <v>0.6</v>
       </c>
       <c r="I24" t="s">
         <v>33</v>
@@ -1218,112 +1250,174 @@
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F25" s="2">
         <v>3</v>
       </c>
       <c r="G25" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="2"/>
-        <v>0.375</v>
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="2">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2">
         <v>7</v>
       </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" ref="H26" si="3">(F26/G26)</f>
-        <v>0.5</v>
+      <c r="H26" s="3">
+        <f t="shared" si="1"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
+      <c r="A27" s="2">
+        <v>18</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2">
         <v>8</v>
       </c>
-      <c r="H27" s="1">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
+      <c r="H27" s="3">
+        <f t="shared" si="1"/>
+        <v>0.375</v>
       </c>
       <c r="I27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="I29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>15</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F30" s="2">
         <v>1</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G30" s="2">
         <v>8</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="2"/>
+      <c r="H30" s="3">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="D29" s="4"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.3">
       <c r="H31" s="1"/>
     </row>
+    <row r="32" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="B32" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:I28">
-    <sortCondition descending="1" ref="F22:F28"/>
-    <sortCondition ref="G22:G28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:I30">
+    <sortCondition descending="1" ref="F20:F30"/>
+    <sortCondition ref="G20:G30"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2 I32:I1048576 I18:I19" xr:uid="{1E6226B8-A8D1-4D7A-9B0F-FAA90AAF118D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2 I33:I1048576 I18:I19" xr:uid="{1E6226B8-A8D1-4D7A-9B0F-FAA90AAF118D}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1331,7 +1425,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I20:I31 I3:I16</xm:sqref>
+          <xm:sqref>I3:I16 I20:I32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>